<commit_message>
Changes for New UI Prod
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC40_Adding_MultipleItems_QuickOrder.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC40_Adding_MultipleItems_QuickOrder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749F4094-D171-4A3D-8553-950B5143ED8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95BD5F2-0577-4804-8468-44DD71289601}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Testdata" sheetId="12" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TC40_Adding_MultipleItems_Quick!$A$1:$E$95</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TC40_Adding_MultipleItems_Quick!$A$1:$E$96</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="76">
   <si>
     <t>TestCase</t>
   </si>
@@ -692,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93"/>
+      <selection activeCell="B90" sqref="B90:B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1803,7 +1803,7 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3"/>
-      <c r="B91" s="7" t="s">
+      <c r="B91" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C91" s="6" t="s">
@@ -1816,7 +1816,7 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="5"/>
-      <c r="B92" s="6" t="s">
+      <c r="B92" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C92" s="6"/>
@@ -1826,43 +1826,52 @@
     <row r="93" spans="1:5">
       <c r="A93" s="5"/>
       <c r="B93" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D93" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E93" s="6" t="s">
-        <v>73</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C93" s="6"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="5"/>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="5"/>
-      <c r="B94" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C94" s="5" t="s">
-        <v>36</v>
+      <c r="B94" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E94" s="5"/>
+      <c r="E94" s="6" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="5"/>
-      <c r="B95" s="6" t="s">
+      <c r="B95" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E95" s="5"/>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="5"/>
+      <c r="B96" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C95" s="5" t="s">
+      <c r="C96" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D95" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E95" s="5"/>
+      <c r="D96" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E96" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -2124,12 +2133,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100599AB90ED4ADBD46B68D7A0832AE2D34" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4d93929aa8d4e603f371af1ff5e0b517">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e6243fcc-5e87-4459-985d-7491a55b4be2" xmlns:ns3="904b644c-3cf7-40e5-b5a5-e101a1ff52b5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="17e9716027504630c423500e26042861" ns2:_="" ns3:_="">
     <xsd:import namespace="e6243fcc-5e87-4459-985d-7491a55b4be2"/>
@@ -2340,6 +2343,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2350,23 +2359,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="904b644c-3cf7-40e5-b5a5-e101a1ff52b5"/>
-    <ds:schemaRef ds:uri="e6243fcc-5e87-4459-985d-7491a55b4be2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CAE325E-5F3B-4FE5-B026-F899F4FA3755}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2385,6 +2377,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="904b644c-3cf7-40e5-b5a5-e101a1ff52b5"/>
+    <ds:schemaRef ds:uri="e6243fcc-5e87-4459-985d-7491a55b4be2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
   <ds:schemaRefs>

</xml_diff>